<commit_message>
add python script for hypothesis test
</commit_message>
<xml_diff>
--- a/Results_tdd/tests_timings.xlsx
+++ b/Results_tdd/tests_timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\IdeaProjects\spring_modulith_tdd\Results_tdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026FD9F7-EC61-4F1C-AFE0-E64533F7A76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611AF536-5D9D-488A-8092-FF950031C1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0BA9F846-8496-4F9B-81FF-42C4360FDE34}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{0BA9F846-8496-4F9B-81FF-42C4360FDE34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,11 +188,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -546,7 +545,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,21 +561,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -585,10 +584,10 @@
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -597,137 +596,137 @@
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>0.33200000000000002</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>1.26</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>1.665</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>1.0840000000000001</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>0.38</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="1">
         <v>8.452</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="1">
         <v>1.704</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>13.871</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>0.33300000000000002</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>1.242</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="1">
         <v>1.6579999999999999</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>1.1359999999999999</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>0.38100000000000001</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="1">
         <v>8.282</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="1">
         <v>1.708</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>14.068</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>0.33600000000000002</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>1.2589999999999999</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>1.657</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>1.1060000000000001</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>0.376</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>9.0009999999999994</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="1">
         <v>1.6990000000000001</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>14.105</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>0.34399999999999997</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>1.25</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="1">
         <v>1.6619999999999999</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>1.1120000000000001</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>0.38500000000000001</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>8.407</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="1">
         <v>1.704</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>14.034000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>0.32700000000000001</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>1.254</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>1.665</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>1.1020000000000001</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>0.375</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <v>8.3879999999999999</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>1.71</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>13.666</v>
       </c>
     </row>
@@ -742,38 +741,14 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <f>AVERAGE(A3:A7)</f>
-        <v>0.33440000000000003</v>
-      </c>
-      <c r="B9" s="1">
-        <f t="shared" ref="B9:H9" si="0">AVERAGE(B3:B7)</f>
-        <v>1.2529999999999997</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>1.6614</v>
-      </c>
-      <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>1.1080000000000001</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
-        <v>0.37940000000000002</v>
-      </c>
-      <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>8.5059999999999985</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7049999999999996</v>
-      </c>
-      <c r="H9" s="1">
-        <f t="shared" si="0"/>
-        <v>13.9488</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>